<commit_message>
Add outlier detection module and general improvements.
</commit_message>
<xml_diff>
--- a/Result/Performance/performance_classic.xlsx
+++ b/Result/Performance/performance_classic.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -521,29 +521,29 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>233/509</t>
+          <t>225/509</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0.7725321888412017</v>
+        <v>0.7822222222222223</v>
       </c>
       <c r="G2" t="n">
-        <v>0.72</v>
+        <v>0.704</v>
       </c>
       <c r="H2" t="n">
-        <v>0.77</v>
+        <v>0.773</v>
       </c>
       <c r="I2" t="n">
-        <v>0.745</v>
+        <v>0.741</v>
       </c>
       <c r="J2" t="n">
         <v>0.758</v>
       </c>
       <c r="K2" t="n">
-        <v>0.758</v>
+        <v>0.757</v>
       </c>
       <c r="L2" t="n">
-        <v>0.7576833976833977</v>
+        <v>0.7574054054054054</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
@@ -572,29 +572,29 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>320/509</t>
+          <t>307/509</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.759375</v>
+        <v>0.758957654723127</v>
       </c>
       <c r="G3" t="n">
-        <v>0.8556338028169014</v>
+        <v>0.8204225352112676</v>
       </c>
       <c r="H3" t="n">
-        <v>0.715</v>
+        <v>0.707</v>
       </c>
       <c r="I3" t="n">
-        <v>0.805</v>
+        <v>0.788</v>
       </c>
       <c r="J3" t="n">
-        <v>0.768</v>
+        <v>0.754</v>
       </c>
       <c r="K3" t="n">
-        <v>0.76</v>
+        <v>0.748</v>
       </c>
       <c r="L3" t="n">
-        <v>0.7567057902973395</v>
+        <v>0.7457668231611894</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -623,29 +623,29 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>204/509</t>
+          <t>201/509</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0.7549019607843137</v>
+        <v>0.736318407960199</v>
       </c>
       <c r="G4" t="n">
-        <v>0.652542372881356</v>
+        <v>0.6271186440677966</v>
       </c>
       <c r="H4" t="n">
-        <v>0.772</v>
+        <v>0.757</v>
       </c>
       <c r="I4" t="n">
-        <v>0.7</v>
+        <v>0.677</v>
       </c>
       <c r="J4" t="n">
-        <v>0.741</v>
+        <v>0.723</v>
       </c>
       <c r="K4" t="n">
-        <v>0.736</v>
+        <v>0.717</v>
       </c>
       <c r="L4" t="n">
-        <v>0.7346960948655864</v>
+        <v>0.7164897249643012</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
@@ -678,25 +678,25 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.7839506172839507</v>
+        <v>0.7962962962962963</v>
       </c>
       <c r="G5" t="n">
-        <v>0.5799086757990868</v>
+        <v>0.589041095890411</v>
       </c>
       <c r="H5" t="n">
-        <v>0.801</v>
+        <v>0.8070000000000001</v>
       </c>
       <c r="I5" t="n">
-        <v>0.667</v>
+        <v>0.677</v>
       </c>
       <c r="J5" t="n">
-        <v>0.75</v>
+        <v>0.758</v>
       </c>
       <c r="K5" t="n">
-        <v>0.734</v>
+        <v>0.742</v>
       </c>
       <c r="L5" t="n">
-        <v>0.7296095103133364</v>
+        <v>0.7376239962210676</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
@@ -725,29 +725,29 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>168/509</t>
+          <t>165/509</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>0.7976190476190477</v>
+        <v>0.8181818181818182</v>
       </c>
       <c r="G6" t="n">
-        <v>0.6320754716981132</v>
+        <v>0.6367924528301887</v>
       </c>
       <c r="H6" t="n">
-        <v>0.824</v>
+        <v>0.833</v>
       </c>
       <c r="I6" t="n">
-        <v>0.705</v>
+        <v>0.716</v>
       </c>
       <c r="J6" t="n">
-        <v>0.78</v>
+        <v>0.79</v>
       </c>
       <c r="K6" t="n">
-        <v>0.765</v>
+        <v>0.775</v>
       </c>
       <c r="L6" t="n">
-        <v>0.7587986786099994</v>
+        <v>0.7678911759100439</v>
       </c>
       <c r="M6" t="inlineStr">
         <is>
@@ -776,29 +776,29 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>171/509</t>
+          <t>176/509</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>0.8011695906432749</v>
+        <v>0.8068181818181818</v>
       </c>
       <c r="G7" t="n">
-        <v>0.6682926829268293</v>
+        <v>0.6926829268292682</v>
       </c>
       <c r="H7" t="n">
-        <v>0.841</v>
+        <v>0.848</v>
       </c>
       <c r="I7" t="n">
-        <v>0.729</v>
+        <v>0.745</v>
       </c>
       <c r="J7" t="n">
-        <v>0.8</v>
+        <v>0.8090000000000001</v>
       </c>
       <c r="K7" t="n">
-        <v>0.785</v>
+        <v>0.797</v>
       </c>
       <c r="L7" t="n">
-        <v>0.7782252888318357</v>
+        <v>0.7904204107830552</v>
       </c>
       <c r="M7" t="inlineStr">
         <is>
@@ -827,29 +827,29 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>329/509</t>
+          <t>325/509</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>0.7781155015197568</v>
+        <v>0.7569230769230769</v>
       </c>
       <c r="G8" t="n">
-        <v>0.847682119205298</v>
+        <v>0.8145695364238411</v>
       </c>
       <c r="H8" t="n">
-        <v>0.6929999999999999</v>
+        <v>0.655</v>
       </c>
       <c r="I8" t="n">
-        <v>0.8110000000000001</v>
+        <v>0.785</v>
       </c>
       <c r="J8" t="n">
-        <v>0.766</v>
+        <v>0.735</v>
       </c>
       <c r="K8" t="n">
-        <v>0.752</v>
+        <v>0.72</v>
       </c>
       <c r="L8" t="n">
-        <v>0.7475125571871901</v>
+        <v>0.7164635121732732</v>
       </c>
       <c r="M8" t="inlineStr">
         <is>
@@ -878,29 +878,29 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>193/509</t>
+          <t>194/509</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>0.7979274611398963</v>
+        <v>0.8195876288659794</v>
       </c>
       <c r="G9" t="n">
-        <v>0.6724890829694323</v>
+        <v>0.6943231441048034</v>
       </c>
       <c r="H9" t="n">
-        <v>0.8090000000000001</v>
+        <v>0.824</v>
       </c>
       <c r="I9" t="n">
-        <v>0.73</v>
+        <v>0.752</v>
       </c>
       <c r="J9" t="n">
-        <v>0.776</v>
+        <v>0.794</v>
       </c>
       <c r="K9" t="n">
-        <v>0.769</v>
+        <v>0.788</v>
       </c>
       <c r="L9" t="n">
-        <v>0.766601684341859</v>
+        <v>0.7846615720524017</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>

</xml_diff>